<commit_message>
The table has been updated.
</commit_message>
<xml_diff>
--- a/Star_Table.xlsx
+++ b/Star_Table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t xml:space="preserve">Star Name</t>
   </si>
@@ -49,6 +49,12 @@
     <t xml:space="preserve">E N14</t>
   </si>
   <si>
+    <t xml:space="preserve">E o16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E N20</t>
+  </si>
+  <si>
     <t xml:space="preserve">15MsunNOROTNOML</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
     <t xml:space="preserve">30Msun_MEDSTRIP</t>
   </si>
   <si>
+    <t xml:space="preserve">30Msun_HIGHSTRIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">40MsunNOROTNOML</t>
   </si>
   <si>
@@ -139,6 +148,12 @@
     <t xml:space="preserve">40MsunLOWSTRIP</t>
   </si>
   <si>
+    <t xml:space="preserve">40MsunMEDSTIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40MsunHIGHSTRIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">50MsunNOROTNOML</t>
   </si>
   <si>
@@ -160,6 +175,12 @@
     <t xml:space="preserve">50MsunLOWSTRIP</t>
   </si>
   <si>
+    <t xml:space="preserve">50MsunMEDSTRIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50MsunHIGHSTRIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">60MsunNOROTNOML</t>
   </si>
   <si>
@@ -182,6 +203,9 @@
   </si>
   <si>
     <t xml:space="preserve">60MsunMEDSTRIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60MsunHIGHSTRIP</t>
   </si>
 </sst>
 </file>
@@ -196,6 +220,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -277,16 +302,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K53" activeCellId="0" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,10 +342,16 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>15</v>
@@ -343,7 +374,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>15</v>
@@ -366,7 +397,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>15</v>
@@ -389,7 +420,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>15</v>
@@ -412,7 +443,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>15</v>
@@ -435,7 +466,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>15</v>
@@ -458,7 +489,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>15</v>
@@ -481,7 +512,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>15</v>
@@ -504,7 +535,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>15</v>
@@ -527,7 +558,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>20</v>
@@ -550,7 +581,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>20</v>
@@ -573,7 +604,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>20</v>
@@ -596,7 +627,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>20</v>
@@ -619,7 +650,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>20</v>
@@ -642,7 +673,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>20</v>
@@ -665,7 +696,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>20</v>
@@ -688,7 +719,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>30</v>
@@ -711,7 +742,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>30</v>
@@ -734,7 +765,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>30</v>
@@ -757,7 +788,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>30</v>
@@ -783,7 +814,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>30</v>
@@ -806,7 +837,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>30</v>
@@ -829,7 +860,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>30</v>
@@ -855,7 +886,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
@@ -881,30 +912,36 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>40</v>
+        <v>3.280753</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>765.293406</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0.674458</v>
+        <v>3.280753</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.305532</v>
+        <v>0.047657</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.423925</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0.50434</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.01803</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>40</v>
@@ -913,21 +950,21 @@
         <v>0</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>21.012453</v>
+        <v>40</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>751.957429</v>
+        <v>765.293406</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0.621235</v>
+        <v>0.674458</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.358845</v>
+        <v>0.305532</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>40</v>
@@ -936,427 +973,430 @@
         <v>0</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>22.800345</v>
+        <v>21.012453</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>962.088279</v>
+        <v>751.957429</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>0.687111</v>
+        <v>0.621235</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.310881</v>
+        <v>0.358845</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>40</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>20.57945</v>
+        <v>22.800345</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>711.652055</v>
+        <v>962.088279</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0.590211</v>
+        <v>0.687111</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>0.389904</v>
+        <v>0.310881</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>40</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>20.597183</v>
+        <v>20.57945</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>462.516827</v>
+        <v>711.652055</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.525698</v>
+        <v>0.590211</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0.454573</v>
+        <v>0.389904</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>40</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>12.880412</v>
+        <v>20.597183</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>1.870159</v>
+        <v>462.516827</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0.525698</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0.980612</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>0.012583</v>
+        <v>0.454573</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>40</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>19.459834</v>
+        <v>12.880412</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>355.753352</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>0.358811</v>
+        <v>1.870159</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0.62171</v>
+        <v>0.980612</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>0.012299</v>
+        <v>0.012583</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>50</v>
+        <v>19.459834</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>692.850828</v>
+        <v>355.753352</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0.646551</v>
+        <v>0.358811</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0.333498</v>
+        <v>0.62171</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0.012299</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>26.663442</v>
+        <v>15.804195</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>627.468731</v>
+        <v>2.384053</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>0.591362</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>0.388796</v>
+        <v>0.980602</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0.012669</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>28.327327</v>
+        <v>8.279869</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>639.75996</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <v>0.668157</v>
-      </c>
-      <c r="G35" s="0" t="n">
-        <v>0.329843</v>
+        <v>0.206381</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.210759</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>0.756786</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>0.020633</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>24.761829</v>
+        <v>50</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>497.968712</v>
+        <v>692.850828</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>0.5634</v>
+        <v>0.646551</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0.416802</v>
+        <v>0.333498</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>24.960687</v>
+        <v>26.663442</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>4.537156</v>
+        <v>627.468731</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>0.142382</v>
+        <v>0.591362</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0.838192</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>0.012687</v>
+        <v>0.388796</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>16.588272</v>
+        <v>28.327327</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1.109683</v>
+        <v>639.75996</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0.668157</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0.950139</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>0.026485</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>0.011001</v>
+        <v>0.329843</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>21.480579</v>
+        <v>24.761829</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>150.393218</v>
+        <v>497.968712</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>0.297374</v>
+        <v>0.5634</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0.683187</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>0.012567</v>
+        <v>0.416802</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>60</v>
+        <v>24.960687</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>866.057688</v>
+        <v>4.537156</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>0.63548</v>
+        <v>0.142382</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0.344592</v>
+        <v>0.838192</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0.012687</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>32.423658</v>
+        <v>16.588272</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>658.242722</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>0.538102</v>
+        <v>1.109683</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0.442132</v>
+        <v>0.950139</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0.026485</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0.011001</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>34.591019</v>
+        <v>21.480579</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>738.267507</v>
+        <v>150.393218</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>0.648231</v>
+        <v>0.297374</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>0.349775</v>
+        <v>0.683187</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0.012567</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>30.898658</v>
+        <v>9.951926</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>575.942128</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>0.495159</v>
+        <v>3.11817</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.485142</v>
+        <v>0.980609</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0.012628</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="C44" s="0" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>27.307617</v>
+        <v>8.265231</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>4.613449</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>0.132578</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>0.848001</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>0.012693</v>
+        <v>0.241938</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.195634</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>0.772988</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>0.024063</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>60</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>25.258299</v>
+        <v>60</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>1.608915</v>
+        <v>866.057688</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0.63548</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.980613</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>0.012638</v>
+        <v>0.344592</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>60</v>
@@ -1365,24 +1405,21 @@
         <v>0</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>26.435051</v>
+        <v>32.423658</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>382.373206</v>
+        <v>658.242722</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>0.381024</v>
+        <v>0.538102</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.599517</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>0.012421</v>
+        <v>0.442132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>60</v>
@@ -1391,16 +1428,166 @@
         <v>0</v>
       </c>
       <c r="D47" s="0" t="n">
+        <v>34.591019</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>738.267507</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0.648231</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0.349775</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>30.898658</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>575.942128</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0.495159</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0.485142</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>27.307617</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>4.613449</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0.132578</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>0.848001</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0.012693</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>25.258299</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>1.608915</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0.980613</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0.012638</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>26.435051</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>382.373206</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0.381024</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0.599517</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0.012421</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="n">
         <v>19.985565</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E52" s="0" t="n">
         <v>2.320877</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G52" s="0" t="n">
         <v>0.980609</v>
       </c>
-      <c r="I47" s="0" t="n">
+      <c r="I52" s="0" t="n">
         <v>0.012653</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>10.945186</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.312794</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.014956</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.224488</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>0.735127</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>0.019083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>